<commit_message>
Added Target Start and End Dates
</commit_message>
<xml_diff>
--- a/Change Log.xlsx
+++ b/Change Log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Serial No.</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>Initial Version</t>
+  </si>
+  <si>
+    <t>Project Plan</t>
+  </si>
+  <si>
+    <t>Added the Target Start and End dates</t>
   </si>
 </sst>
 </file>
@@ -439,7 +445,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -449,7 +455,7 @@
     <col min="3" max="3" width="17.26953125" style="9" customWidth="1"/>
     <col min="4" max="4" width="39.1796875" customWidth="1"/>
     <col min="5" max="5" width="19.7265625" customWidth="1"/>
-    <col min="6" max="6" width="31.26953125" customWidth="1"/>
+    <col min="6" max="6" width="33.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -493,12 +499,24 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>43144</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.78749999999999998</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>

</xml_diff>

<commit_message>
Added "reviewed by" column
Added entries 3,4
</commit_message>
<xml_diff>
--- a/Change Log.xlsx
+++ b/Change Log.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Member1\Documents\SEIS732\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\New folder (3)\Course Material UST\Sem 5-Spr2018\Data Warehousing\Assignments\ATeam1\A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{BF0E2EAA-86FA-4EDD-9FCA-72F850488F9A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19152" windowHeight="6864" xr2:uid="{BF0E2EAA-86FA-4EDD-9FCA-72F850488F9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Serial No.</t>
   </si>
@@ -57,6 +57,18 @@
   </si>
   <si>
     <t>Added the Target Start and End dates</t>
+  </si>
+  <si>
+    <t>Team_04_M1_D3_Communication_Policy</t>
+  </si>
+  <si>
+    <t>Team_04_M1_D5_Liaison</t>
+  </si>
+  <si>
+    <t>2100-Prerana</t>
+  </si>
+  <si>
+    <t>Reviewed By</t>
   </si>
 </sst>
 </file>
@@ -442,23 +454,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A5D38B-77DE-4CA8-815D-F3D57B5B5080}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.90625" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="39.1796875" customWidth="1"/>
-    <col min="5" max="5" width="19.7265625" customWidth="1"/>
-    <col min="6" max="6" width="33.54296875" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="39.21875" customWidth="1"/>
+    <col min="5" max="6" width="19.77734375" customWidth="1"/>
+    <col min="7" max="7" width="33.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="29.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -475,10 +487,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -494,11 +509,12 @@
       <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -514,193 +530,241 @@
       <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>43145</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.78125</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>43146</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.78194444444444444</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="5"/>
       <c r="C6" s="8"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="5"/>
       <c r="C7" s="8"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="5"/>
       <c r="C8" s="8"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
       <c r="C9" s="8"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
       <c r="C10" s="8"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
       <c r="C11" s="8"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="8"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
       <c r="C13" s="8"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
       <c r="C14" s="8"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="5"/>
       <c r="C15" s="8"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="5"/>
       <c r="C16" s="8"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="5"/>
       <c r="C17" s="8"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="5"/>
       <c r="C18" s="8"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="5"/>
       <c r="C19" s="8"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="5"/>
       <c r="C20" s="8"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="5"/>
       <c r="C21" s="8"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="5"/>
       <c r="C22" s="8"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
       <c r="C23" s="8"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
       <c r="C24" s="8"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="5"/>
       <c r="C25" s="8"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="5"/>
       <c r="C26" s="8"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Project Plan tasks
</commit_message>
<xml_diff>
--- a/Change Log.xlsx
+++ b/Change Log.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\New folder (3)\Course Material UST\Sem 5-Spr2018\Data Warehousing\Assignments\ATeam1\A3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Member1\Documents\SEIS732\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19152" windowHeight="6864" xr2:uid="{BF0E2EAA-86FA-4EDD-9FCA-72F850488F9A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{BF0E2EAA-86FA-4EDD-9FCA-72F850488F9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Serial No.</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Reviewed By</t>
+  </si>
+  <si>
+    <t>Added the Task details and Dates</t>
   </si>
 </sst>
 </file>
@@ -457,20 +460,20 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="39.21875" customWidth="1"/>
-    <col min="5" max="6" width="19.77734375" customWidth="1"/>
-    <col min="7" max="7" width="33.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.90625" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="39.1796875" customWidth="1"/>
+    <col min="5" max="6" width="19.81640625" customWidth="1"/>
+    <col min="7" max="7" width="33.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="29.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -493,7 +496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -514,7 +517,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -535,7 +538,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -556,7 +559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -577,16 +580,30 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>43144</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.81388888888888899</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="5"/>
       <c r="C7" s="8"/>
@@ -595,7 +612,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="5"/>
       <c r="C8" s="8"/>
@@ -604,7 +621,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
       <c r="C9" s="8"/>
@@ -613,7 +630,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
       <c r="C10" s="8"/>
@@ -622,7 +639,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
       <c r="C11" s="8"/>
@@ -631,7 +648,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="8"/>
@@ -640,7 +657,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
       <c r="C13" s="8"/>
@@ -649,7 +666,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
       <c r="C14" s="8"/>
@@ -658,7 +675,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="5"/>
       <c r="C15" s="8"/>
@@ -667,7 +684,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="5"/>
       <c r="C16" s="8"/>
@@ -676,7 +693,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="5"/>
       <c r="C17" s="8"/>
@@ -685,7 +702,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="5"/>
       <c r="C18" s="8"/>
@@ -694,7 +711,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="5"/>
       <c r="C19" s="8"/>
@@ -703,7 +720,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="5"/>
       <c r="C20" s="8"/>
@@ -712,7 +729,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="5"/>
       <c r="C21" s="8"/>
@@ -721,7 +738,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="5"/>
       <c r="C22" s="8"/>
@@ -730,7 +747,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
       <c r="C23" s="8"/>
@@ -739,7 +756,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
       <c r="C24" s="8"/>
@@ -748,7 +765,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="5"/>
       <c r="C25" s="8"/>
@@ -757,7 +774,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="5"/>
       <c r="C26" s="8"/>

</xml_diff>

<commit_message>
Added log for M1D4
changed date modified for sr no. 3,4
</commit_message>
<xml_diff>
--- a/Change Log.xlsx
+++ b/Change Log.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Member1\Documents\SEIS732\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\New folder (3)\Course Material UST\Sem 5-Spr2018\Data Warehousing\Assignments\ATeam1\A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{BF0E2EAA-86FA-4EDD-9FCA-72F850488F9A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19152" windowHeight="6864" xr2:uid="{BF0E2EAA-86FA-4EDD-9FCA-72F850488F9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Serial No.</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Added the Task details and Dates</t>
+  </si>
+  <si>
+    <t>Team_04_M1_D4_Tool_Policy</t>
   </si>
 </sst>
 </file>
@@ -460,20 +463,20 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.90625" customWidth="1"/>
-    <col min="2" max="2" width="17.1796875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="39.1796875" customWidth="1"/>
-    <col min="5" max="6" width="19.81640625" customWidth="1"/>
-    <col min="7" max="7" width="33.54296875" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="39.21875" customWidth="1"/>
+    <col min="5" max="6" width="19.77734375" customWidth="1"/>
+    <col min="7" max="7" width="33.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="29.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -496,7 +499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -517,7 +520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -538,12 +541,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="5">
-        <v>43145</v>
+        <v>43144</v>
       </c>
       <c r="C4" s="8">
         <v>0.78125</v>
@@ -559,12 +562,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <v>43146</v>
+        <v>43144</v>
       </c>
       <c r="C5" s="8">
         <v>0.78194444444444444</v>
@@ -580,7 +583,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -603,16 +606,28 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5">
+        <v>43144</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="5"/>
       <c r="C8" s="8"/>
@@ -621,7 +636,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
       <c r="C9" s="8"/>
@@ -630,7 +645,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
       <c r="C10" s="8"/>
@@ -639,7 +654,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
       <c r="C11" s="8"/>
@@ -648,7 +663,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="8"/>
@@ -657,7 +672,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
       <c r="C13" s="8"/>
@@ -666,7 +681,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
       <c r="C14" s="8"/>
@@ -675,7 +690,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="5"/>
       <c r="C15" s="8"/>
@@ -684,7 +699,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="5"/>
       <c r="C16" s="8"/>
@@ -693,7 +708,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="5"/>
       <c r="C17" s="8"/>
@@ -702,7 +717,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="5"/>
       <c r="C18" s="8"/>
@@ -711,7 +726,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="5"/>
       <c r="C19" s="8"/>
@@ -720,7 +735,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="5"/>
       <c r="C20" s="8"/>
@@ -729,7 +744,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="5"/>
       <c r="C21" s="8"/>
@@ -738,7 +753,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="5"/>
       <c r="C22" s="8"/>
@@ -747,7 +762,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
       <c r="C23" s="8"/>
@@ -756,7 +771,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
       <c r="C24" s="8"/>
@@ -765,7 +780,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="5"/>
       <c r="C25" s="8"/>
@@ -774,7 +789,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="5"/>
       <c r="C26" s="8"/>

</xml_diff>